<commit_message>
Excel Configuration for Add Book API
</commit_message>
<xml_diff>
--- a/src/test/java/resources/TestData.xlsx
+++ b/src/test/java/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\restAssuredWorkSpace\src\test\java\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE23A03-F46E-4BF4-821B-05CACF07C531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F608BD-8AFC-473F-A9EE-5F6E3043C861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="7270" xr2:uid="{1A1579F4-8FBB-4CEB-9C9B-2DA280A02D26}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1A1579F4-8FBB-4CEB-9C9B-2DA280A02D26}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,19 +47,19 @@
     <t>Data3</t>
   </si>
   <si>
-    <t xml:space="preserve">BookName </t>
-  </si>
-  <si>
-    <t>Aisle</t>
-  </si>
-  <si>
-    <t>Author</t>
-  </si>
-  <si>
-    <t>GetBook</t>
-  </si>
-  <si>
     <t>Data4</t>
+  </si>
+  <si>
+    <t>AddBook</t>
+  </si>
+  <si>
+    <t>MongoDB</t>
+  </si>
+  <si>
+    <t>ty</t>
+  </si>
+  <si>
+    <t>Ajit Naidu</t>
   </si>
 </sst>
 </file>
@@ -95,8 +95,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,7 +417,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -437,24 +440,24 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>1234</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Parameters to getData
</commit_message>
<xml_diff>
--- a/src/test/java/resources/TestData.xlsx
+++ b/src/test/java/resources/TestData.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\restAssuredWorkSpace\src\test\java\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F608BD-8AFC-473F-A9EE-5F6E3043C861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EEA8385-B7AB-4AF8-A2B6-701D721C2511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1A1579F4-8FBB-4CEB-9C9B-2DA280A02D26}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="LibraryAPI" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,18 +38,6 @@
     <t>TestCaseName</t>
   </si>
   <si>
-    <t>Data1</t>
-  </si>
-  <si>
-    <t>Data2</t>
-  </si>
-  <si>
-    <t>Data3</t>
-  </si>
-  <si>
-    <t>Data4</t>
-  </si>
-  <si>
     <t>AddBook</t>
   </si>
   <si>
@@ -60,6 +48,18 @@
   </si>
   <si>
     <t>Ajit Naidu</t>
+  </si>
+  <si>
+    <t>BookName</t>
+  </si>
+  <si>
+    <t>ISBN</t>
+  </si>
+  <si>
+    <t>ISLE</t>
+  </si>
+  <si>
+    <t>Author</t>
   </si>
 </sst>
 </file>
@@ -417,7 +417,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -431,33 +431,33 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1">
         <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>